<commit_message>
daily push 19 jan
</commit_message>
<xml_diff>
--- a/vix_spread_daily_log.xlsx
+++ b/vix_spread_daily_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1081,6 +1081,54 @@
         <v>2168</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2026-01-20 00:59:45</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="D14" t="n">
+        <v>115</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1102</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1217</v>
+      </c>
+      <c r="I14" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="J14" t="n">
+        <v>2</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="N14" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
push 20 jan csv log
</commit_message>
<xml_diff>
--- a/vix_spread_daily_log.xlsx
+++ b/vix_spread_daily_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1129,6 +1129,54 @@
         <v>3</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2026-01-21</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2026-01-21 00:00:14</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="D15" t="n">
+        <v>25799</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="F15" t="n">
+        <v>6676</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="H15" t="n">
+        <v>32475</v>
+      </c>
+      <c r="I15" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="J15" t="n">
+        <v>15836</v>
+      </c>
+      <c r="K15" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="L15" t="n">
+        <v>530</v>
+      </c>
+      <c r="M15" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="N15" t="n">
+        <v>16366</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
git and auto run automation
</commit_message>
<xml_diff>
--- a/vix_spread_daily_log.xlsx
+++ b/vix_spread_daily_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1177,6 +1177,54 @@
         <v>16366</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2026-01-22 21:30:41</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="D16" t="n">
+        <v>4</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="F16" t="n">
+        <v>21</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.7500000000000001</v>
+      </c>
+      <c r="H16" t="n">
+        <v>25</v>
+      </c>
+      <c r="I16" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J16" t="n">
+        <v>129</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="L16" t="n">
+        <v>1658</v>
+      </c>
+      <c r="M16" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="N16" t="n">
+        <v>1787</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>